<commit_message>
load info from file
</commit_message>
<xml_diff>
--- a/test/summary_grp.xlsx
+++ b/test/summary_grp.xlsx
@@ -42,10 +42,10 @@
     <t>Upper 95% CI</t>
   </si>
   <si>
-    <t>C12</t>
+    <t>c12</t>
   </si>
   <si>
-    <t>C13</t>
+    <t>c13</t>
   </si>
 </sst>
 </file>

</xml_diff>